<commit_message>
changed Brakepressure to 16bit
</commit_message>
<xml_diff>
--- a/EDBC_TY22evo.xlsx
+++ b/EDBC_TY22evo.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847C32C9-7A3A-43B2-BCC7-009AB8C7F93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMS" sheetId="13" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -362,12 +363,15 @@
   </si>
   <si>
     <t>TS_RDY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -435,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -443,34 +447,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -479,7 +456,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -761,44 +747,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -825,36 +811,36 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="K2" s="9"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>200</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="5" t="s">
         <v>57</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="1" t="s">
         <v>60</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -863,14 +849,12 @@
       <c r="K3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    </row>
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>201</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -879,16 +863,16 @@
       <c r="D4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="5" t="s">
         <v>59</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -900,84 +884,82 @@
       <c r="K4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    </row>
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>202</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>203</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="8" t="s">
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="4" t="s">
         <v>106</v>
       </c>
     </row>
@@ -993,44 +975,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1057,15 +1039,15 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1095,14 +1077,12 @@
       <c r="K3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1132,14 +1112,12 @@
       <c r="K4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1169,16 +1147,15 @@
       <c r="K5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    </row>
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1206,14 +1183,12 @@
         <v>98</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    </row>
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1241,35 +1216,33 @@
         <v>103</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    </row>
+    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1296,15 +1269,15 @@
       <c r="J10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="K10" s="9"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1334,14 +1307,12 @@
       <c r="K11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    </row>
+    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1371,14 +1342,12 @@
       <c r="K12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    </row>
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1408,16 +1377,15 @@
       <c r="K13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    </row>
+    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1445,14 +1413,12 @@
         <v>98</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    </row>
+    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1480,8 +1446,6 @@
         <v>103</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1498,44 +1462,44 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1562,15 +1526,15 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="K2" s="9"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>400</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1600,37 +1564,36 @@
       <c r="K3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    </row>
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-    </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1657,73 +1620,71 @@
       <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="K6" s="9"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>410</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>100</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    </row>
+    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1750,15 +1711,15 @@
       <c r="J10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="K10" s="9"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>420</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1788,10 +1749,14 @@
       <c r="K11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M11" s="3"/>
+    </row>
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1811,44 +1776,44 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1875,15 +1840,15 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="K2" s="9"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>500</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1913,16 +1878,15 @@
       <c r="K3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    </row>
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>501</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1950,8 +1914,6 @@
         <v>16</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1965,44 +1927,44 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C7" sqref="C7:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2029,15 +1991,15 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="K2" s="9"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>600</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2067,14 +2029,12 @@
       <c r="K3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    </row>
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>601</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2104,14 +2064,12 @@
       <c r="K4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2141,14 +2099,12 @@
       <c r="K5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2179,11 +2135,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>100</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2214,11 +2170,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>100</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2261,44 +2217,44 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2325,15 +2281,15 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="K2" s="9"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>700</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2361,14 +2317,12 @@
         <v>16</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    </row>
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>701</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2396,35 +2350,33 @@
         <v>16</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    </row>
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="12" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2451,15 +2403,15 @@
       <c r="J7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="K7" s="9"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>710</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>100</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2487,14 +2439,12 @@
         <v>16</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    </row>
+    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>711</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2522,35 +2472,33 @@
         <v>16</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    </row>
+    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2577,15 +2525,15 @@
       <c r="J12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="K12" s="9"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+    </row>
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>720</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>100</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2613,14 +2561,12 @@
         <v>16</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    </row>
+    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>721</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2648,35 +2594,33 @@
         <v>16</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-    </row>
-    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    </row>
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2703,15 +2647,15 @@
       <c r="J17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K17" s="12"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-    </row>
-    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="K17" s="9"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+    </row>
+    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>730</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>100</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2739,14 +2683,12 @@
         <v>16</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+    </row>
+    <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>731</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2774,23 +2716,21 @@
         <v>16</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="K1:M2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="K6:M7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="K11:M12"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:J16"/>
     <mergeCell ref="K16:M17"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:M2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="K6:M7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2798,44 +2738,44 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2862,15 +2802,15 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="K2" s="9"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>796</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2898,14 +2838,12 @@
         <v>16</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    </row>
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>797</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2933,14 +2871,12 @@
         <v>64</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    </row>
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>798</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2968,14 +2904,12 @@
         <v>74</v>
       </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    </row>
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>799</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -3003,8 +2937,6 @@
         <v>16</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3018,44 +2950,44 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K4" sqref="A4:K5"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3082,15 +3014,15 @@
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="K2" s="9"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>800</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -3120,8 +3052,6 @@
       <c r="K3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
changed SWC ID to 0x750
</commit_message>
<xml_diff>
--- a/EDBC_TY22evo.xlsx
+++ b/EDBC_TY22evo.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D96FAD-37D8-4F86-8644-3583633354ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AMS" sheetId="13" r:id="rId1"/>
@@ -371,7 +370,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -747,19 +746,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
@@ -780,7 +779,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +814,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>200</v>
       </c>
@@ -850,7 +849,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>201</v>
       </c>
@@ -885,7 +884,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>202</v>
       </c>
@@ -920,7 +919,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>203</v>
       </c>
@@ -955,7 +954,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>105</v>
       </c>
@@ -975,19 +974,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>78</v>
       </c>
@@ -1008,7 +1007,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1042,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -1078,7 +1077,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>89</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>91</v>
       </c>
@@ -1151,7 +1150,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>92</v>
       </c>
@@ -1184,7 +1183,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>93</v>
       </c>
@@ -1217,7 +1216,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>79</v>
       </c>
@@ -1238,7 +1237,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1273,7 +1272,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
@@ -1308,7 +1307,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>89</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
@@ -1381,7 +1380,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -1414,7 +1413,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
@@ -1462,19 +1461,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -1495,7 +1494,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1530,7 +1529,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>400</v>
       </c>
@@ -1568,7 +1567,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
@@ -1589,7 +1588,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +1623,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>410</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1680,7 +1679,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1715,7 +1714,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>420</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F13" s="1" t="s">
         <v>112</v>
       </c>
@@ -1776,19 +1775,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
@@ -1809,7 +1808,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1844,7 +1843,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>500</v>
       </c>
@@ -1882,7 +1881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>501</v>
       </c>
@@ -1927,19 +1926,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>44</v>
       </c>
@@ -1960,7 +1959,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +1994,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>600</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>601</v>
       </c>
@@ -2065,7 +2064,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>83</v>
       </c>
@@ -2100,7 +2099,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>83</v>
       </c>
@@ -2135,7 +2134,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>82</v>
       </c>
@@ -2170,7 +2169,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -2217,19 +2216,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>48</v>
       </c>
@@ -2250,7 +2249,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2285,7 +2284,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>700</v>
       </c>
@@ -2318,7 +2317,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>701</v>
       </c>
@@ -2351,7 +2350,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
@@ -2372,7 +2371,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2407,7 +2406,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>710</v>
       </c>
@@ -2440,7 +2439,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>711</v>
       </c>
@@ -2473,7 +2472,7 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>50</v>
       </c>
@@ -2494,7 +2493,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -2529,7 +2528,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>720</v>
       </c>
@@ -2562,7 +2561,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>721</v>
       </c>
@@ -2595,7 +2594,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -2616,7 +2615,7 @@
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
     </row>
-    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -2651,7 +2650,7 @@
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
     </row>
-    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>730</v>
       </c>
@@ -2684,7 +2683,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>731</v>
       </c>
@@ -2719,18 +2718,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="K1:M2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="K6:M7"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="K11:M12"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:J16"/>
     <mergeCell ref="K16:M17"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:M2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="K6:M7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2738,19 +2737,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
@@ -2771,7 +2770,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2806,7 +2805,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>796</v>
       </c>
@@ -2839,7 +2838,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>797</v>
       </c>
@@ -2872,7 +2871,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>798</v>
       </c>
@@ -2905,7 +2904,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>799</v>
       </c>
@@ -2950,19 +2949,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
@@ -2983,7 +2982,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3018,9 +3017,9 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="B3" s="3">
         <v>100</v>

</xml_diff>

<commit_message>
Update on AMS CAN
</commit_message>
<xml_diff>
--- a/EDBC_TY22evo.xlsx
+++ b/EDBC_TY22evo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="AMS" sheetId="13" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="AIM EVO 5" sheetId="16" r:id="rId7"/>
     <sheet name="SWC" sheetId="4" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -749,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -952,6 +952,9 @@
       </c>
       <c r="K6" s="2" t="s">
         <v>28</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -978,7 +981,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I3" sqref="I3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1930,7 +1933,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2220,7 +2223,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2718,18 +2721,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="K11:M12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="K16:M17"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="K1:M2"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="K6:M7"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="K11:M12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:J16"/>
-    <mergeCell ref="K16:M17"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2952,7 +2955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>